<commit_message>
Fixed Schematic and Updated PCB
</commit_message>
<xml_diff>
--- a/Documentation/Component Glossary.xlsx
+++ b/Documentation/Component Glossary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishav\Documents\GitHub\9w_LED_PCB\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BFF669-B9B4-4E53-909D-F8ED09071F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7685DEE-4F41-487A-83D3-672A94B239E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{2AE41DF5-7B5A-4E92-9D0C-918A9F32479A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Radial-cylinderical</t>
   </si>
   <si>
-    <t>Transformer wound</t>
-  </si>
-  <si>
     <t>MOV-07D511K 320V 100pF 10%</t>
   </si>
   <si>
@@ -255,19 +252,31 @@
     <t>Ceramic 103</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01uF 1KV </t>
-  </si>
-  <si>
     <t>Connect either c6 or c5</t>
   </si>
   <si>
-    <t>Maintains power on falling edge of current signal - Flicker free continuous operation</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NC if C6 is NC</t>
   </si>
   <si>
     <t>List of Materials</t>
+  </si>
+  <si>
+    <t>7mH NTL-</t>
+  </si>
+  <si>
+    <t>Transformer wound type Inductor. Maintains power on falling edge of current signal - Flicker free continuous operation</t>
+  </si>
+  <si>
+    <t>2.1mH</t>
+  </si>
+  <si>
+    <t>320V/100pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01uF 400V </t>
+  </si>
+  <si>
+    <t>220nF 50V</t>
   </si>
 </sst>
 </file>
@@ -420,10 +429,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -732,7 +741,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -742,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6044EE84-06AC-4B0E-95D4-8C23F45A7574}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,15 +766,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
+      <c r="A1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -787,7 +796,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -804,10 +813,10 @@
         <v>32</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G3" s="7"/>
     </row>
@@ -825,10 +834,10 @@
         <v>39</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="7"/>
     </row>
@@ -843,16 +852,16 @@
         <v>33</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -869,7 +878,7 @@
         <v>40</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="7"/>
@@ -888,7 +897,7 @@
         <v>40</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="7"/>
@@ -904,12 +913,14 @@
         <v>33</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>83</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -923,12 +934,12 @@
         <v>33</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -979,13 +990,13 @@
         <v>42</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1002,13 +1013,13 @@
         <v>42</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1022,14 +1033,14 @@
         <v>38</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1046,14 +1057,16 @@
         <v>44</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -1064,16 +1077,16 @@
         <v>36</v>
       </c>
       <c r="D16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>45</v>
-      </c>
       <c r="G16" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1087,11 +1100,13 @@
         <v>37</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>53</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="F17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="7"/>
     </row>
@@ -1106,10 +1121,10 @@
         <v>35</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="10">
         <v>334</v>
@@ -1127,10 +1142,10 @@
         <v>35</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="10">
         <v>334</v>
@@ -1148,10 +1163,10 @@
         <v>35</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F20" s="10">
         <v>473</v>
@@ -1169,10 +1184,10 @@
         <v>35</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F21" s="10">
         <v>243</v>
@@ -1190,10 +1205,10 @@
         <v>35</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="10">
         <v>154</v>
@@ -1211,10 +1226,10 @@
         <v>35</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="10">
         <v>154</v>
@@ -1232,10 +1247,10 @@
         <v>35</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24" s="10">
         <v>211</v>
@@ -1253,12 +1268,12 @@
         <v>35</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1272,13 +1287,13 @@
         <v>35</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G26" s="7"/>
     </row>
@@ -1293,13 +1308,13 @@
         <v>35</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G27" s="8"/>
     </row>

</xml_diff>